<commit_message>
aggiornamenti minimi interfaccia - extra trasferta spostato nel json
</commit_message>
<xml_diff>
--- a/static/report_commessa_compilato.xlsx
+++ b/static/report_commessa_compilato.xlsx
@@ -471,7 +471,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -500,8 +500,9 @@
           <t>Costo totale</t>
         </is>
       </c>
-      <c r="E1" t="n">
-        <v>304</v>
+      <c r="E1" s="4">
+        <f>SUM(F12:F500)</f>
+        <v/>
       </c>
       <c r="G1" s="6" t="n"/>
     </row>
@@ -521,8 +522,9 @@
           <t>Ore lavorate</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>7.5</v>
+      <c r="E2" s="4">
+        <f>SUM(C12:C500)</f>
+        <v/>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="5">
@@ -639,10 +641,8 @@
           <t>Alberto Calmini</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C12" t="n">
+        <v>4</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -669,10 +669,8 @@
           <t>Alberto Calmini</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
+      <c r="C13" t="n">
+        <v>3.5</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Aggiunto sort by date negli inserimenti - miglioramenti minimi grafica
</commit_message>
<xml_diff>
--- a/static/report_commessa_compilato.xlsx
+++ b/static/report_commessa_compilato.xlsx
@@ -468,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
@@ -492,7 +492,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>0001</t>
+          <t>0004</t>
         </is>
       </c>
       <c r="D1" s="6" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mega commessa</t>
+          <t>Commesa a caso</t>
         </is>
       </c>
       <c r="D2" s="6" t="inlineStr">
@@ -535,7 +535,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pippo Baudo</t>
+          <t>Golamixin</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>14/07/2021</t>
+          <t>10/05/2023</t>
         </is>
       </c>
     </row>
@@ -559,7 +559,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>20/02/2022</t>
+          <t>13/06/2023</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" ht="12.8" customHeight="1" s="5">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="10" ht="12.8" customHeight="1" s="5">
@@ -633,7 +633,7 @@
     <row r="12" ht="12.8" customHeight="1" s="5">
       <c r="A12" s="7" t="inlineStr">
         <is>
-          <t>12/10/2021</t>
+          <t>09/06/2023</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -651,17 +651,17 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Stress Analysis</t>
+          <t>Altro</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>68</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" ht="12.8" customHeight="1" s="5">
       <c r="A13" s="7" t="inlineStr">
         <is>
-          <t>15/01/2022</t>
+          <t>12/06/2023</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -670,24 +670,77 @@
         </is>
       </c>
       <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Stress Analysis</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" ht="12.8" customHeight="1" s="5">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>12/06/2023</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Alberto Calmini</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Altro</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>13/06/2023</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Alberto Calmini</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
         <v>3.5</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Stress Analysis</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Supporti</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>236</v>
       </c>
-    </row>
-    <row r="14" ht="12.8" customHeight="1" s="5">
-      <c r="A14" s="7" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>